<commit_message>
found some more spelling mistakes and renamed studycode variable accordingly
</commit_message>
<xml_diff>
--- a/02_data/cleandata/idstocheck.xlsx
+++ b/02_data/cleandata/idstocheck.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="395">
   <si>
     <t xml:space="preserve">studycode</t>
   </si>
@@ -494,7 +494,7 @@
     <t xml:space="preserve">transition to psychosis</t>
   </si>
   <si>
-    <t xml:space="preserve">kristensenandcadenhead_2007</t>
+    <t xml:space="preserve">kristensen_2007</t>
   </si>
   <si>
     <t xml:space="preserve">auther_2012</t>
@@ -521,9 +521,6 @@
     <t xml:space="preserve">dragt_2012</t>
   </si>
   <si>
-    <t xml:space="preserve">kristensen_2007</t>
-  </si>
-  <si>
     <t xml:space="preserve">dragt_2010</t>
   </si>
   <si>
@@ -542,7 +539,7 @@
     <t xml:space="preserve">berger_2016</t>
   </si>
   <si>
-    <t xml:space="preserve">bloemen_2010</t>
+    <t xml:space="preserve">bloemen_2009</t>
   </si>
   <si>
     <t xml:space="preserve">bousman_2013</t>
@@ -941,7 +938,7 @@
     <t xml:space="preserve">hadden_2018</t>
   </si>
   <si>
-    <t xml:space="preserve">ouellett-plamondon_2017</t>
+    <t xml:space="preserve">ouellet-plamondon_2017</t>
   </si>
   <si>
     <t xml:space="preserve">seddon_2016</t>
@@ -1556,7 +1553,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3">
@@ -1570,7 +1567,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4">
@@ -1584,7 +1581,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5">
@@ -1598,7 +1595,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6">
@@ -1612,7 +1609,7 @@
         <v>6</v>
       </c>
       <c r="D6" t="n">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7">
@@ -1626,7 +1623,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8">
@@ -1668,7 +1665,7 @@
         <v>15</v>
       </c>
       <c r="D10" t="n">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11">
@@ -1682,7 +1679,7 @@
         <v>15</v>
       </c>
       <c r="D11" t="n">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12">
@@ -1710,7 +1707,7 @@
         <v>15</v>
       </c>
       <c r="D13" t="n">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14">
@@ -1724,7 +1721,7 @@
         <v>15</v>
       </c>
       <c r="D14" t="n">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15">
@@ -1738,7 +1735,7 @@
         <v>15</v>
       </c>
       <c r="D15" t="n">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="16">
@@ -1766,7 +1763,7 @@
         <v>15</v>
       </c>
       <c r="D17" t="n">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18">
@@ -1864,7 +1861,7 @@
         <v>28</v>
       </c>
       <c r="D24" t="n">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25">
@@ -1892,7 +1889,7 @@
         <v>28</v>
       </c>
       <c r="D26" t="n">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27">
@@ -1906,7 +1903,7 @@
         <v>28</v>
       </c>
       <c r="D27" t="n">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28">
@@ -1934,7 +1931,7 @@
         <v>28</v>
       </c>
       <c r="D29" t="n">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30">
@@ -1962,7 +1959,7 @@
         <v>38</v>
       </c>
       <c r="D31" t="n">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="32">
@@ -2074,7 +2071,7 @@
         <v>28</v>
       </c>
       <c r="D39" t="n">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="40">
@@ -2088,7 +2085,7 @@
         <v>28</v>
       </c>
       <c r="D40" t="n">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="41">
@@ -2116,7 +2113,7 @@
         <v>28</v>
       </c>
       <c r="D42" t="n">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="43">
@@ -2130,7 +2127,7 @@
         <v>38</v>
       </c>
       <c r="D43" t="n">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="44">
@@ -2158,7 +2155,7 @@
         <v>38</v>
       </c>
       <c r="D45" t="n">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="46">
@@ -2172,7 +2169,7 @@
         <v>38</v>
       </c>
       <c r="D46" t="n">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47">
@@ -2200,7 +2197,7 @@
         <v>41</v>
       </c>
       <c r="D48" t="n">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="49">
@@ -2214,7 +2211,7 @@
         <v>61</v>
       </c>
       <c r="D49" t="n">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="50">
@@ -2256,7 +2253,7 @@
         <v>61</v>
       </c>
       <c r="D52" t="n">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53">
@@ -2298,7 +2295,7 @@
         <v>61</v>
       </c>
       <c r="D55" t="n">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56">
@@ -2340,7 +2337,7 @@
         <v>61</v>
       </c>
       <c r="D58" t="n">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="59">
@@ -2354,7 +2351,7 @@
         <v>61</v>
       </c>
       <c r="D59" t="n">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="60">
@@ -2368,7 +2365,7 @@
         <v>61</v>
       </c>
       <c r="D60" t="n">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="61">
@@ -2382,7 +2379,7 @@
         <v>61</v>
       </c>
       <c r="D61" t="n">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="62">
@@ -2396,7 +2393,7 @@
         <v>61</v>
       </c>
       <c r="D62" t="n">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="63">
@@ -2410,7 +2407,7 @@
         <v>76</v>
       </c>
       <c r="D63" t="n">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="64">
@@ -2424,7 +2421,7 @@
         <v>76</v>
       </c>
       <c r="D64" t="n">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="65">
@@ -2438,7 +2435,7 @@
         <v>76</v>
       </c>
       <c r="D65" t="n">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="66">
@@ -2466,7 +2463,7 @@
         <v>76</v>
       </c>
       <c r="D67" t="n">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="68">
@@ -2522,7 +2519,7 @@
         <v>76</v>
       </c>
       <c r="D71" t="n">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="72">
@@ -2536,7 +2533,7 @@
         <v>76</v>
       </c>
       <c r="D72" t="n">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="73">
@@ -2592,7 +2589,7 @@
         <v>90</v>
       </c>
       <c r="D76" t="n">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="77">
@@ -2662,7 +2659,7 @@
         <v>90</v>
       </c>
       <c r="D81" t="n">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="82">
@@ -2844,7 +2841,7 @@
         <v>99</v>
       </c>
       <c r="D94" t="n">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="95">
@@ -2858,7 +2855,7 @@
         <v>99</v>
       </c>
       <c r="D95" t="n">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="96">
@@ -2872,7 +2869,7 @@
         <v>99</v>
       </c>
       <c r="D96" t="n">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="97">
@@ -2886,7 +2883,7 @@
         <v>99</v>
       </c>
       <c r="D97" t="n">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="98">
@@ -2900,7 +2897,7 @@
         <v>99</v>
       </c>
       <c r="D98" t="n">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="99">
@@ -2914,7 +2911,7 @@
         <v>99</v>
       </c>
       <c r="D99" t="n">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="100">
@@ -2928,7 +2925,7 @@
         <v>99</v>
       </c>
       <c r="D100" t="n">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="101">
@@ -2942,7 +2939,7 @@
         <v>99</v>
       </c>
       <c r="D101" t="n">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="102">
@@ -2956,7 +2953,7 @@
         <v>99</v>
       </c>
       <c r="D102" t="n">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="103">
@@ -2970,7 +2967,7 @@
         <v>99</v>
       </c>
       <c r="D103" t="n">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="104">
@@ -2984,7 +2981,7 @@
         <v>99</v>
       </c>
       <c r="D104" t="n">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="105">
@@ -2998,7 +2995,7 @@
         <v>99</v>
       </c>
       <c r="D105" t="n">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="106">
@@ -3082,7 +3079,7 @@
         <v>99</v>
       </c>
       <c r="D111" t="n">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="112">
@@ -3096,7 +3093,7 @@
         <v>99</v>
       </c>
       <c r="D112" t="n">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="113">
@@ -3110,7 +3107,7 @@
         <v>99</v>
       </c>
       <c r="D113" t="n">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="114">
@@ -3124,7 +3121,7 @@
         <v>99</v>
       </c>
       <c r="D114" t="n">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="115">
@@ -3208,7 +3205,7 @@
         <v>99</v>
       </c>
       <c r="D120" t="n">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="121">
@@ -3222,7 +3219,7 @@
         <v>99</v>
       </c>
       <c r="D121" t="n">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="122">
@@ -3236,7 +3233,7 @@
         <v>99</v>
       </c>
       <c r="D122" t="n">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="123">
@@ -3250,7 +3247,7 @@
         <v>99</v>
       </c>
       <c r="D123" t="n">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="124">
@@ -3264,7 +3261,7 @@
         <v>99</v>
       </c>
       <c r="D124" t="n">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="125">
@@ -3278,7 +3275,7 @@
         <v>99</v>
       </c>
       <c r="D125" t="n">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="126">
@@ -3348,7 +3345,7 @@
         <v>99</v>
       </c>
       <c r="D130" t="n">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="131">
@@ -3390,7 +3387,7 @@
         <v>99</v>
       </c>
       <c r="D133" t="n">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="134">
@@ -3404,7 +3401,7 @@
         <v>99</v>
       </c>
       <c r="D134" t="n">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="135">
@@ -3432,7 +3429,7 @@
         <v>99</v>
       </c>
       <c r="D136" t="n">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="137">
@@ -3446,7 +3443,7 @@
         <v>99</v>
       </c>
       <c r="D137" t="n">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="138">
@@ -3488,7 +3485,7 @@
         <v>99</v>
       </c>
       <c r="D140" t="n">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="141">
@@ -3516,7 +3513,7 @@
         <v>159</v>
       </c>
       <c r="D142" t="n">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="143">
@@ -3544,7 +3541,7 @@
         <v>159</v>
       </c>
       <c r="D144" t="n">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="145">
@@ -3614,7 +3611,7 @@
         <v>159</v>
       </c>
       <c r="D149" t="n">
-        <v>170</v>
+        <v>89</v>
       </c>
     </row>
     <row r="150">
@@ -3628,7 +3625,7 @@
         <v>159</v>
       </c>
       <c r="D150" t="n">
-        <v>89</v>
+        <v>47</v>
       </c>
     </row>
     <row r="151">
@@ -3642,7 +3639,7 @@
         <v>159</v>
       </c>
       <c r="D151" t="n">
-        <v>47</v>
+        <v>202</v>
       </c>
     </row>
     <row r="152">
@@ -3656,7 +3653,7 @@
         <v>159</v>
       </c>
       <c r="D152" t="n">
-        <v>203</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153">
@@ -3670,7 +3667,7 @@
         <v>159</v>
       </c>
       <c r="D153" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="154">
@@ -3684,7 +3681,7 @@
         <v>159</v>
       </c>
       <c r="D154" t="n">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="155">
@@ -3698,7 +3695,7 @@
         <v>159</v>
       </c>
       <c r="D155" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="156">
@@ -3712,7 +3709,7 @@
         <v>159</v>
       </c>
       <c r="D156" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="157">
@@ -3726,7 +3723,7 @@
         <v>159</v>
       </c>
       <c r="D157" t="n">
-        <v>42</v>
+        <v>76</v>
       </c>
     </row>
     <row r="158">
@@ -3740,7 +3737,7 @@
         <v>159</v>
       </c>
       <c r="D158" t="n">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="159">
@@ -3754,7 +3751,7 @@
         <v>159</v>
       </c>
       <c r="D159" t="n">
-        <v>81</v>
+        <v>107</v>
       </c>
     </row>
     <row r="160">
@@ -3768,7 +3765,7 @@
         <v>159</v>
       </c>
       <c r="D160" t="n">
-        <v>107</v>
+        <v>172</v>
       </c>
     </row>
     <row r="161">
@@ -3782,7 +3779,7 @@
         <v>159</v>
       </c>
       <c r="D161" t="n">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="162">
@@ -3796,7 +3793,7 @@
         <v>159</v>
       </c>
       <c r="D162" t="n">
-        <v>175</v>
+        <v>215</v>
       </c>
     </row>
     <row r="163">
@@ -3810,7 +3807,7 @@
         <v>159</v>
       </c>
       <c r="D163" t="n">
-        <v>216</v>
+        <v>249</v>
       </c>
     </row>
     <row r="164">
@@ -3824,7 +3821,7 @@
         <v>159</v>
       </c>
       <c r="D164" t="n">
-        <v>250</v>
+        <v>277</v>
       </c>
     </row>
     <row r="165">
@@ -3838,7 +3835,7 @@
         <v>159</v>
       </c>
       <c r="D165" t="n">
-        <v>278</v>
+        <v>320</v>
       </c>
     </row>
     <row r="166">
@@ -3852,7 +3849,7 @@
         <v>159</v>
       </c>
       <c r="D166" t="n">
-        <v>321</v>
+        <v>337</v>
       </c>
     </row>
     <row r="167">
@@ -3863,24 +3860,24 @@
         <v>5</v>
       </c>
       <c r="C167" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="D167" t="n">
-        <v>338</v>
+        <v>166</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
+        <v>189</v>
+      </c>
+      <c r="B168" t="s">
+        <v>5</v>
+      </c>
+      <c r="C168" t="s">
         <v>188</v>
       </c>
-      <c r="B168" t="s">
-        <v>5</v>
-      </c>
-      <c r="C168" t="s">
-        <v>189</v>
-      </c>
       <c r="D168" t="n">
-        <v>166</v>
+        <v>231</v>
       </c>
     </row>
     <row r="169">
@@ -3891,24 +3888,24 @@
         <v>5</v>
       </c>
       <c r="C169" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D169" t="n">
-        <v>232</v>
+        <v>48</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="s">
+        <v>192</v>
+      </c>
+      <c r="B170" t="s">
+        <v>5</v>
+      </c>
+      <c r="C170" t="s">
         <v>191</v>
       </c>
-      <c r="B170" t="s">
-        <v>5</v>
-      </c>
-      <c r="C170" t="s">
-        <v>192</v>
-      </c>
       <c r="D170" t="n">
-        <v>48</v>
+        <v>206</v>
       </c>
     </row>
     <row r="171">
@@ -3919,10 +3916,10 @@
         <v>5</v>
       </c>
       <c r="C171" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D171" t="n">
-        <v>207</v>
+        <v>216</v>
       </c>
     </row>
     <row r="172">
@@ -3933,10 +3930,10 @@
         <v>5</v>
       </c>
       <c r="C172" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D172" t="n">
-        <v>217</v>
+        <v>316</v>
       </c>
     </row>
     <row r="173">
@@ -3944,27 +3941,27 @@
         <v>195</v>
       </c>
       <c r="B173" t="s">
-        <v>5</v>
+        <v>196</v>
       </c>
       <c r="C173" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D173" t="n">
-        <v>317</v>
+        <v>119</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="s">
+        <v>198</v>
+      </c>
+      <c r="B174" t="s">
         <v>196</v>
       </c>
-      <c r="B174" t="s">
+      <c r="C174" t="s">
         <v>197</v>
       </c>
-      <c r="C174" t="s">
-        <v>198</v>
-      </c>
       <c r="D174" t="n">
-        <v>119</v>
+        <v>330</v>
       </c>
     </row>
     <row r="175">
@@ -3972,27 +3969,27 @@
         <v>199</v>
       </c>
       <c r="B175" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C175" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D175" t="n">
-        <v>331</v>
+        <v>4</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="s">
+        <v>202</v>
+      </c>
+      <c r="B176" t="s">
         <v>200</v>
       </c>
-      <c r="B176" t="s">
+      <c r="C176" t="s">
         <v>201</v>
       </c>
-      <c r="C176" t="s">
-        <v>202</v>
-      </c>
       <c r="D176" t="n">
-        <v>4</v>
+        <v>134</v>
       </c>
     </row>
     <row r="177">
@@ -4000,13 +3997,13 @@
         <v>203</v>
       </c>
       <c r="B177" t="s">
+        <v>200</v>
+      </c>
+      <c r="C177" t="s">
         <v>201</v>
       </c>
-      <c r="C177" t="s">
-        <v>202</v>
-      </c>
       <c r="D177" t="n">
-        <v>134</v>
+        <v>238</v>
       </c>
     </row>
     <row r="178">
@@ -4014,13 +4011,13 @@
         <v>204</v>
       </c>
       <c r="B178" t="s">
+        <v>200</v>
+      </c>
+      <c r="C178" t="s">
         <v>201</v>
       </c>
-      <c r="C178" t="s">
-        <v>202</v>
-      </c>
       <c r="D178" t="n">
-        <v>239</v>
+        <v>255</v>
       </c>
     </row>
     <row r="179">
@@ -4028,27 +4025,27 @@
         <v>205</v>
       </c>
       <c r="B179" t="s">
+        <v>206</v>
+      </c>
+      <c r="C179" t="s">
         <v>201</v>
       </c>
-      <c r="C179" t="s">
-        <v>202</v>
-      </c>
       <c r="D179" t="n">
-        <v>256</v>
+        <v>300</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B180" t="s">
-        <v>207</v>
+        <v>5</v>
       </c>
       <c r="C180" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D180" t="n">
-        <v>301</v>
+        <v>80</v>
       </c>
     </row>
     <row r="181">
@@ -4056,27 +4053,27 @@
         <v>208</v>
       </c>
       <c r="B181" t="s">
-        <v>5</v>
+        <v>209</v>
       </c>
       <c r="C181" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="D181" t="n">
-        <v>80</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="s">
+        <v>211</v>
+      </c>
+      <c r="B182" t="s">
         <v>209</v>
       </c>
-      <c r="B182" t="s">
+      <c r="C182" t="s">
         <v>210</v>
       </c>
-      <c r="C182" t="s">
-        <v>211</v>
-      </c>
       <c r="D182" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="183">
@@ -4084,13 +4081,13 @@
         <v>212</v>
       </c>
       <c r="B183" t="s">
+        <v>209</v>
+      </c>
+      <c r="C183" t="s">
         <v>210</v>
       </c>
-      <c r="C183" t="s">
-        <v>211</v>
-      </c>
       <c r="D183" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="184">
@@ -4098,13 +4095,13 @@
         <v>213</v>
       </c>
       <c r="B184" t="s">
+        <v>209</v>
+      </c>
+      <c r="C184" t="s">
         <v>210</v>
       </c>
-      <c r="C184" t="s">
-        <v>211</v>
-      </c>
       <c r="D184" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="185">
@@ -4112,13 +4109,13 @@
         <v>214</v>
       </c>
       <c r="B185" t="s">
+        <v>209</v>
+      </c>
+      <c r="C185" t="s">
         <v>210</v>
       </c>
-      <c r="C185" t="s">
-        <v>211</v>
-      </c>
       <c r="D185" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="186">
@@ -4126,13 +4123,13 @@
         <v>215</v>
       </c>
       <c r="B186" t="s">
+        <v>209</v>
+      </c>
+      <c r="C186" t="s">
         <v>210</v>
       </c>
-      <c r="C186" t="s">
-        <v>211</v>
-      </c>
       <c r="D186" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="187">
@@ -4140,13 +4137,13 @@
         <v>216</v>
       </c>
       <c r="B187" t="s">
+        <v>209</v>
+      </c>
+      <c r="C187" t="s">
         <v>210</v>
       </c>
-      <c r="C187" t="s">
-        <v>211</v>
-      </c>
       <c r="D187" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="188">
@@ -4154,13 +4151,13 @@
         <v>217</v>
       </c>
       <c r="B188" t="s">
+        <v>209</v>
+      </c>
+      <c r="C188" t="s">
         <v>210</v>
       </c>
-      <c r="C188" t="s">
-        <v>211</v>
-      </c>
       <c r="D188" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="189">
@@ -4168,13 +4165,13 @@
         <v>218</v>
       </c>
       <c r="B189" t="s">
+        <v>209</v>
+      </c>
+      <c r="C189" t="s">
         <v>210</v>
       </c>
-      <c r="C189" t="s">
-        <v>211</v>
-      </c>
       <c r="D189" t="n">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="190">
@@ -4182,13 +4179,13 @@
         <v>219</v>
       </c>
       <c r="B190" t="s">
+        <v>209</v>
+      </c>
+      <c r="C190" t="s">
         <v>210</v>
       </c>
-      <c r="C190" t="s">
-        <v>211</v>
-      </c>
       <c r="D190" t="n">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="191">
@@ -4196,13 +4193,13 @@
         <v>220</v>
       </c>
       <c r="B191" t="s">
+        <v>209</v>
+      </c>
+      <c r="C191" t="s">
         <v>210</v>
       </c>
-      <c r="C191" t="s">
-        <v>211</v>
-      </c>
       <c r="D191" t="n">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="192">
@@ -4210,13 +4207,13 @@
         <v>221</v>
       </c>
       <c r="B192" t="s">
+        <v>209</v>
+      </c>
+      <c r="C192" t="s">
         <v>210</v>
       </c>
-      <c r="C192" t="s">
-        <v>211</v>
-      </c>
       <c r="D192" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="193">
@@ -4224,13 +4221,13 @@
         <v>222</v>
       </c>
       <c r="B193" t="s">
+        <v>209</v>
+      </c>
+      <c r="C193" t="s">
         <v>210</v>
       </c>
-      <c r="C193" t="s">
-        <v>211</v>
-      </c>
       <c r="D193" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="194">
@@ -4238,13 +4235,13 @@
         <v>223</v>
       </c>
       <c r="B194" t="s">
+        <v>209</v>
+      </c>
+      <c r="C194" t="s">
         <v>210</v>
       </c>
-      <c r="C194" t="s">
-        <v>211</v>
-      </c>
       <c r="D194" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="195">
@@ -4252,13 +4249,13 @@
         <v>224</v>
       </c>
       <c r="B195" t="s">
+        <v>209</v>
+      </c>
+      <c r="C195" t="s">
         <v>210</v>
       </c>
-      <c r="C195" t="s">
-        <v>211</v>
-      </c>
       <c r="D195" t="n">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="196">
@@ -4266,13 +4263,13 @@
         <v>225</v>
       </c>
       <c r="B196" t="s">
+        <v>209</v>
+      </c>
+      <c r="C196" t="s">
         <v>210</v>
       </c>
-      <c r="C196" t="s">
-        <v>211</v>
-      </c>
       <c r="D196" t="n">
-        <v>71</v>
+        <v>97</v>
       </c>
     </row>
     <row r="197">
@@ -4280,13 +4277,13 @@
         <v>226</v>
       </c>
       <c r="B197" t="s">
+        <v>209</v>
+      </c>
+      <c r="C197" t="s">
         <v>210</v>
       </c>
-      <c r="C197" t="s">
-        <v>211</v>
-      </c>
       <c r="D197" t="n">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="198">
@@ -4294,13 +4291,13 @@
         <v>227</v>
       </c>
       <c r="B198" t="s">
+        <v>209</v>
+      </c>
+      <c r="C198" t="s">
         <v>210</v>
       </c>
-      <c r="C198" t="s">
-        <v>211</v>
-      </c>
       <c r="D198" t="n">
-        <v>111</v>
+        <v>132</v>
       </c>
     </row>
     <row r="199">
@@ -4308,13 +4305,13 @@
         <v>228</v>
       </c>
       <c r="B199" t="s">
+        <v>209</v>
+      </c>
+      <c r="C199" t="s">
         <v>210</v>
       </c>
-      <c r="C199" t="s">
-        <v>211</v>
-      </c>
       <c r="D199" t="n">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="200">
@@ -4322,13 +4319,13 @@
         <v>229</v>
       </c>
       <c r="B200" t="s">
+        <v>209</v>
+      </c>
+      <c r="C200" t="s">
         <v>210</v>
       </c>
-      <c r="C200" t="s">
-        <v>211</v>
-      </c>
       <c r="D200" t="n">
-        <v>141</v>
+        <v>150</v>
       </c>
     </row>
     <row r="201">
@@ -4336,13 +4333,13 @@
         <v>230</v>
       </c>
       <c r="B201" t="s">
+        <v>209</v>
+      </c>
+      <c r="C201" t="s">
         <v>210</v>
       </c>
-      <c r="C201" t="s">
-        <v>211</v>
-      </c>
       <c r="D201" t="n">
-        <v>150</v>
+        <v>159</v>
       </c>
     </row>
     <row r="202">
@@ -4350,13 +4347,13 @@
         <v>231</v>
       </c>
       <c r="B202" t="s">
+        <v>209</v>
+      </c>
+      <c r="C202" t="s">
         <v>210</v>
       </c>
-      <c r="C202" t="s">
-        <v>211</v>
-      </c>
       <c r="D202" t="n">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="203">
@@ -4364,13 +4361,13 @@
         <v>232</v>
       </c>
       <c r="B203" t="s">
+        <v>209</v>
+      </c>
+      <c r="C203" t="s">
         <v>210</v>
       </c>
-      <c r="C203" t="s">
-        <v>211</v>
-      </c>
       <c r="D203" t="n">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="204">
@@ -4378,13 +4375,13 @@
         <v>233</v>
       </c>
       <c r="B204" t="s">
+        <v>209</v>
+      </c>
+      <c r="C204" t="s">
         <v>210</v>
       </c>
-      <c r="C204" t="s">
-        <v>211</v>
-      </c>
       <c r="D204" t="n">
-        <v>163</v>
+        <v>191</v>
       </c>
     </row>
     <row r="205">
@@ -4392,13 +4389,13 @@
         <v>234</v>
       </c>
       <c r="B205" t="s">
+        <v>209</v>
+      </c>
+      <c r="C205" t="s">
         <v>210</v>
       </c>
-      <c r="C205" t="s">
-        <v>211</v>
-      </c>
       <c r="D205" t="n">
-        <v>192</v>
+        <v>199</v>
       </c>
     </row>
     <row r="206">
@@ -4406,13 +4403,13 @@
         <v>235</v>
       </c>
       <c r="B206" t="s">
+        <v>209</v>
+      </c>
+      <c r="C206" t="s">
         <v>210</v>
       </c>
-      <c r="C206" t="s">
-        <v>211</v>
-      </c>
       <c r="D206" t="n">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="207">
@@ -4420,13 +4417,13 @@
         <v>236</v>
       </c>
       <c r="B207" t="s">
+        <v>209</v>
+      </c>
+      <c r="C207" t="s">
         <v>210</v>
       </c>
-      <c r="C207" t="s">
+      <c r="D207" t="n">
         <v>211</v>
-      </c>
-      <c r="D207" t="n">
-        <v>204</v>
       </c>
     </row>
     <row r="208">
@@ -4434,13 +4431,13 @@
         <v>237</v>
       </c>
       <c r="B208" t="s">
+        <v>209</v>
+      </c>
+      <c r="C208" t="s">
         <v>210</v>
       </c>
-      <c r="C208" t="s">
-        <v>211</v>
-      </c>
       <c r="D208" t="n">
-        <v>212</v>
+        <v>217</v>
       </c>
     </row>
     <row r="209">
@@ -4448,13 +4445,13 @@
         <v>238</v>
       </c>
       <c r="B209" t="s">
+        <v>209</v>
+      </c>
+      <c r="C209" t="s">
         <v>210</v>
       </c>
-      <c r="C209" t="s">
-        <v>211</v>
-      </c>
       <c r="D209" t="n">
-        <v>218</v>
+        <v>233</v>
       </c>
     </row>
     <row r="210">
@@ -4462,10 +4459,10 @@
         <v>239</v>
       </c>
       <c r="B210" t="s">
+        <v>209</v>
+      </c>
+      <c r="C210" t="s">
         <v>210</v>
-      </c>
-      <c r="C210" t="s">
-        <v>211</v>
       </c>
       <c r="D210" t="n">
         <v>234</v>
@@ -4476,10 +4473,10 @@
         <v>240</v>
       </c>
       <c r="B211" t="s">
+        <v>209</v>
+      </c>
+      <c r="C211" t="s">
         <v>210</v>
-      </c>
-      <c r="C211" t="s">
-        <v>211</v>
       </c>
       <c r="D211" t="n">
         <v>235</v>
@@ -4490,13 +4487,13 @@
         <v>241</v>
       </c>
       <c r="B212" t="s">
+        <v>209</v>
+      </c>
+      <c r="C212" t="s">
         <v>210</v>
       </c>
-      <c r="C212" t="s">
-        <v>211</v>
-      </c>
       <c r="D212" t="n">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
     <row r="213">
@@ -4504,13 +4501,13 @@
         <v>242</v>
       </c>
       <c r="B213" t="s">
+        <v>209</v>
+      </c>
+      <c r="C213" t="s">
         <v>210</v>
       </c>
-      <c r="C213" t="s">
-        <v>211</v>
-      </c>
       <c r="D213" t="n">
-        <v>242</v>
+        <v>254</v>
       </c>
     </row>
     <row r="214">
@@ -4518,13 +4515,13 @@
         <v>243</v>
       </c>
       <c r="B214" t="s">
+        <v>209</v>
+      </c>
+      <c r="C214" t="s">
         <v>210</v>
       </c>
-      <c r="C214" t="s">
-        <v>211</v>
-      </c>
       <c r="D214" t="n">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="215">
@@ -4532,13 +4529,13 @@
         <v>244</v>
       </c>
       <c r="B215" t="s">
+        <v>209</v>
+      </c>
+      <c r="C215" t="s">
         <v>210</v>
       </c>
-      <c r="C215" t="s">
-        <v>211</v>
-      </c>
       <c r="D215" t="n">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="216">
@@ -4546,13 +4543,13 @@
         <v>245</v>
       </c>
       <c r="B216" t="s">
+        <v>209</v>
+      </c>
+      <c r="C216" t="s">
         <v>210</v>
       </c>
-      <c r="C216" t="s">
-        <v>211</v>
-      </c>
       <c r="D216" t="n">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="217">
@@ -4560,13 +4557,13 @@
         <v>246</v>
       </c>
       <c r="B217" t="s">
+        <v>209</v>
+      </c>
+      <c r="C217" t="s">
         <v>210</v>
       </c>
-      <c r="C217" t="s">
-        <v>211</v>
-      </c>
       <c r="D217" t="n">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
     <row r="218">
@@ -4574,13 +4571,13 @@
         <v>247</v>
       </c>
       <c r="B218" t="s">
+        <v>209</v>
+      </c>
+      <c r="C218" t="s">
         <v>210</v>
       </c>
-      <c r="C218" t="s">
-        <v>211</v>
-      </c>
       <c r="D218" t="n">
-        <v>275</v>
+        <v>284</v>
       </c>
     </row>
     <row r="219">
@@ -4588,13 +4585,13 @@
         <v>248</v>
       </c>
       <c r="B219" t="s">
+        <v>209</v>
+      </c>
+      <c r="C219" t="s">
         <v>210</v>
       </c>
-      <c r="C219" t="s">
-        <v>211</v>
-      </c>
       <c r="D219" t="n">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="220">
@@ -4602,10 +4599,10 @@
         <v>249</v>
       </c>
       <c r="B220" t="s">
+        <v>209</v>
+      </c>
+      <c r="C220" t="s">
         <v>210</v>
-      </c>
-      <c r="C220" t="s">
-        <v>211</v>
       </c>
       <c r="D220" t="n">
         <v>287</v>
@@ -4616,13 +4613,13 @@
         <v>250</v>
       </c>
       <c r="B221" t="s">
+        <v>209</v>
+      </c>
+      <c r="C221" t="s">
         <v>210</v>
       </c>
-      <c r="C221" t="s">
-        <v>211</v>
-      </c>
       <c r="D221" t="n">
-        <v>288</v>
+        <v>295</v>
       </c>
     </row>
     <row r="222">
@@ -4630,13 +4627,13 @@
         <v>251</v>
       </c>
       <c r="B222" t="s">
+        <v>209</v>
+      </c>
+      <c r="C222" t="s">
         <v>210</v>
       </c>
-      <c r="C222" t="s">
-        <v>211</v>
-      </c>
       <c r="D222" t="n">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="223">
@@ -4644,10 +4641,10 @@
         <v>252</v>
       </c>
       <c r="B223" t="s">
+        <v>209</v>
+      </c>
+      <c r="C223" t="s">
         <v>210</v>
-      </c>
-      <c r="C223" t="s">
-        <v>211</v>
       </c>
       <c r="D223" t="n">
         <v>303</v>
@@ -4658,13 +4655,13 @@
         <v>253</v>
       </c>
       <c r="B224" t="s">
+        <v>209</v>
+      </c>
+      <c r="C224" t="s">
         <v>210</v>
       </c>
-      <c r="C224" t="s">
-        <v>211</v>
-      </c>
       <c r="D224" t="n">
-        <v>304</v>
+        <v>327</v>
       </c>
     </row>
     <row r="225">
@@ -4672,13 +4669,13 @@
         <v>254</v>
       </c>
       <c r="B225" t="s">
+        <v>209</v>
+      </c>
+      <c r="C225" t="s">
         <v>210</v>
       </c>
-      <c r="C225" t="s">
-        <v>211</v>
-      </c>
       <c r="D225" t="n">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="226">
@@ -4686,13 +4683,13 @@
         <v>255</v>
       </c>
       <c r="B226" t="s">
+        <v>209</v>
+      </c>
+      <c r="C226" t="s">
         <v>210</v>
       </c>
-      <c r="C226" t="s">
-        <v>211</v>
-      </c>
       <c r="D226" t="n">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="227">
@@ -4700,27 +4697,27 @@
         <v>256</v>
       </c>
       <c r="B227" t="s">
-        <v>210</v>
+        <v>5</v>
       </c>
       <c r="C227" t="s">
-        <v>211</v>
+        <v>257</v>
       </c>
       <c r="D227" t="n">
-        <v>337</v>
+        <v>73</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="s">
+        <v>258</v>
+      </c>
+      <c r="B228" t="s">
+        <v>5</v>
+      </c>
+      <c r="C228" t="s">
         <v>257</v>
       </c>
-      <c r="B228" t="s">
-        <v>5</v>
-      </c>
-      <c r="C228" t="s">
-        <v>258</v>
-      </c>
       <c r="D228" t="n">
-        <v>73</v>
+        <v>298</v>
       </c>
     </row>
     <row r="229">
@@ -4731,10 +4728,10 @@
         <v>5</v>
       </c>
       <c r="C229" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D229" t="n">
-        <v>299</v>
+        <v>18</v>
       </c>
     </row>
     <row r="230">
@@ -4742,27 +4739,27 @@
         <v>260</v>
       </c>
       <c r="B230" t="s">
-        <v>5</v>
+        <v>261</v>
       </c>
       <c r="C230" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D230" t="n">
-        <v>18</v>
+        <v>230</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="s">
+        <v>262</v>
+      </c>
+      <c r="B231" t="s">
         <v>261</v>
       </c>
-      <c r="B231" t="s">
-        <v>262</v>
-      </c>
       <c r="C231" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D231" t="n">
-        <v>231</v>
+        <v>149</v>
       </c>
     </row>
     <row r="232">
@@ -4770,13 +4767,13 @@
         <v>263</v>
       </c>
       <c r="B232" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C232" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D232" t="n">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="233">
@@ -4784,13 +4781,13 @@
         <v>264</v>
       </c>
       <c r="B233" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C233" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D233" t="n">
-        <v>151</v>
+        <v>250</v>
       </c>
     </row>
     <row r="234">
@@ -4798,13 +4795,13 @@
         <v>265</v>
       </c>
       <c r="B234" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C234" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D234" t="n">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="235">
@@ -4812,13 +4809,13 @@
         <v>266</v>
       </c>
       <c r="B235" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C235" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D235" t="n">
-        <v>248</v>
+        <v>101</v>
       </c>
     </row>
     <row r="236">
@@ -4826,13 +4823,13 @@
         <v>267</v>
       </c>
       <c r="B236" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C236" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D236" t="n">
-        <v>101</v>
+        <v>30</v>
       </c>
     </row>
     <row r="237">
@@ -4840,27 +4837,27 @@
         <v>268</v>
       </c>
       <c r="B237" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C237" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="D237" t="n">
-        <v>30</v>
+        <v>264</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="s">
+        <v>271</v>
+      </c>
+      <c r="B238" t="s">
         <v>269</v>
       </c>
-      <c r="B238" t="s">
+      <c r="C238" t="s">
         <v>270</v>
       </c>
-      <c r="C238" t="s">
-        <v>271</v>
-      </c>
       <c r="D238" t="n">
-        <v>265</v>
+        <v>123</v>
       </c>
     </row>
     <row r="239">
@@ -4868,13 +4865,13 @@
         <v>272</v>
       </c>
       <c r="B239" t="s">
+        <v>269</v>
+      </c>
+      <c r="C239" t="s">
         <v>270</v>
       </c>
-      <c r="C239" t="s">
-        <v>271</v>
-      </c>
       <c r="D239" t="n">
-        <v>123</v>
+        <v>178</v>
       </c>
     </row>
     <row r="240">
@@ -4882,13 +4879,13 @@
         <v>273</v>
       </c>
       <c r="B240" t="s">
+        <v>269</v>
+      </c>
+      <c r="C240" t="s">
         <v>270</v>
       </c>
-      <c r="C240" t="s">
-        <v>271</v>
-      </c>
       <c r="D240" t="n">
-        <v>179</v>
+        <v>41</v>
       </c>
     </row>
     <row r="241">
@@ -4896,13 +4893,13 @@
         <v>274</v>
       </c>
       <c r="B241" t="s">
+        <v>269</v>
+      </c>
+      <c r="C241" t="s">
         <v>270</v>
       </c>
-      <c r="C241" t="s">
-        <v>271</v>
-      </c>
       <c r="D241" t="n">
-        <v>41</v>
+        <v>292</v>
       </c>
     </row>
     <row r="242">
@@ -4910,13 +4907,13 @@
         <v>275</v>
       </c>
       <c r="B242" t="s">
+        <v>269</v>
+      </c>
+      <c r="C242" t="s">
         <v>270</v>
       </c>
-      <c r="C242" t="s">
-        <v>271</v>
-      </c>
       <c r="D242" t="n">
-        <v>293</v>
+        <v>236</v>
       </c>
     </row>
     <row r="243">
@@ -4924,13 +4921,13 @@
         <v>276</v>
       </c>
       <c r="B243" t="s">
+        <v>269</v>
+      </c>
+      <c r="C243" t="s">
         <v>270</v>
       </c>
-      <c r="C243" t="s">
-        <v>271</v>
-      </c>
       <c r="D243" t="n">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="244">
@@ -4938,13 +4935,13 @@
         <v>277</v>
       </c>
       <c r="B244" t="s">
+        <v>269</v>
+      </c>
+      <c r="C244" t="s">
         <v>270</v>
       </c>
-      <c r="C244" t="s">
-        <v>271</v>
-      </c>
       <c r="D244" t="n">
-        <v>241</v>
+        <v>281</v>
       </c>
     </row>
     <row r="245">
@@ -4952,13 +4949,13 @@
         <v>278</v>
       </c>
       <c r="B245" t="s">
+        <v>269</v>
+      </c>
+      <c r="C245" t="s">
         <v>270</v>
       </c>
-      <c r="C245" t="s">
-        <v>271</v>
-      </c>
       <c r="D245" t="n">
-        <v>282</v>
+        <v>54</v>
       </c>
     </row>
     <row r="246">
@@ -4966,13 +4963,13 @@
         <v>279</v>
       </c>
       <c r="B246" t="s">
+        <v>269</v>
+      </c>
+      <c r="C246" t="s">
         <v>270</v>
       </c>
-      <c r="C246" t="s">
-        <v>271</v>
-      </c>
       <c r="D246" t="n">
-        <v>54</v>
+        <v>310</v>
       </c>
     </row>
     <row r="247">
@@ -4980,13 +4977,13 @@
         <v>280</v>
       </c>
       <c r="B247" t="s">
+        <v>269</v>
+      </c>
+      <c r="C247" t="s">
         <v>270</v>
       </c>
-      <c r="C247" t="s">
-        <v>271</v>
-      </c>
       <c r="D247" t="n">
-        <v>311</v>
+        <v>145</v>
       </c>
     </row>
     <row r="248">
@@ -4994,27 +4991,27 @@
         <v>281</v>
       </c>
       <c r="B248" t="s">
+        <v>282</v>
+      </c>
+      <c r="C248" t="s">
         <v>270</v>
       </c>
-      <c r="C248" t="s">
-        <v>271</v>
-      </c>
       <c r="D248" t="n">
-        <v>145</v>
+        <v>246</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="s">
+        <v>283</v>
+      </c>
+      <c r="B249" t="s">
         <v>282</v>
       </c>
-      <c r="B249" t="s">
-        <v>283</v>
-      </c>
       <c r="C249" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D249" t="n">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="250">
@@ -5022,13 +5019,13 @@
         <v>284</v>
       </c>
       <c r="B250" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C250" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D250" t="n">
-        <v>249</v>
+        <v>269</v>
       </c>
     </row>
     <row r="251">
@@ -5036,27 +5033,27 @@
         <v>285</v>
       </c>
       <c r="B251" t="s">
-        <v>283</v>
+        <v>5</v>
       </c>
       <c r="C251" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="D251" t="n">
-        <v>270</v>
+        <v>142</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="s">
+        <v>287</v>
+      </c>
+      <c r="B252" t="s">
+        <v>5</v>
+      </c>
+      <c r="C252" t="s">
         <v>286</v>
       </c>
-      <c r="B252" t="s">
-        <v>5</v>
-      </c>
-      <c r="C252" t="s">
-        <v>287</v>
-      </c>
       <c r="D252" t="n">
-        <v>142</v>
+        <v>325</v>
       </c>
     </row>
     <row r="253">
@@ -5067,10 +5064,10 @@
         <v>5</v>
       </c>
       <c r="C253" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D253" t="n">
-        <v>326</v>
+        <v>193</v>
       </c>
     </row>
     <row r="254">
@@ -5078,27 +5075,27 @@
         <v>289</v>
       </c>
       <c r="B254" t="s">
-        <v>5</v>
+        <v>290</v>
       </c>
       <c r="C254" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D254" t="n">
-        <v>194</v>
+        <v>213</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="s">
+        <v>291</v>
+      </c>
+      <c r="B255" t="s">
         <v>290</v>
       </c>
-      <c r="B255" t="s">
-        <v>291</v>
-      </c>
       <c r="C255" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D255" t="n">
-        <v>214</v>
+        <v>260</v>
       </c>
     </row>
     <row r="256">
@@ -5106,13 +5103,13 @@
         <v>292</v>
       </c>
       <c r="B256" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C256" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D256" t="n">
-        <v>261</v>
+        <v>293</v>
       </c>
     </row>
     <row r="257">
@@ -5120,13 +5117,13 @@
         <v>293</v>
       </c>
       <c r="B257" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C257" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D257" t="n">
-        <v>294</v>
+        <v>244</v>
       </c>
     </row>
     <row r="258">
@@ -5134,13 +5131,13 @@
         <v>294</v>
       </c>
       <c r="B258" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C258" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D258" t="n">
-        <v>245</v>
+        <v>261</v>
       </c>
     </row>
     <row r="259">
@@ -5148,13 +5145,13 @@
         <v>295</v>
       </c>
       <c r="B259" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C259" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D259" t="n">
-        <v>262</v>
+        <v>162</v>
       </c>
     </row>
     <row r="260">
@@ -5162,13 +5159,13 @@
         <v>296</v>
       </c>
       <c r="B260" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C260" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D260" t="n">
-        <v>162</v>
+        <v>309</v>
       </c>
     </row>
     <row r="261">
@@ -5176,27 +5173,27 @@
         <v>297</v>
       </c>
       <c r="B261" t="s">
-        <v>291</v>
+        <v>5</v>
       </c>
       <c r="C261" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
       <c r="D261" t="n">
-        <v>310</v>
+        <v>3</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="s">
+        <v>299</v>
+      </c>
+      <c r="B262" t="s">
+        <v>5</v>
+      </c>
+      <c r="C262" t="s">
         <v>298</v>
       </c>
-      <c r="B262" t="s">
-        <v>5</v>
-      </c>
-      <c r="C262" t="s">
-        <v>299</v>
-      </c>
       <c r="D262" t="n">
-        <v>3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="263">
@@ -5207,10 +5204,10 @@
         <v>5</v>
       </c>
       <c r="C263" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D263" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="264">
@@ -5221,10 +5218,10 @@
         <v>5</v>
       </c>
       <c r="C264" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D264" t="n">
-        <v>36</v>
+        <v>61</v>
       </c>
     </row>
     <row r="265">
@@ -5235,10 +5232,10 @@
         <v>5</v>
       </c>
       <c r="C265" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D265" t="n">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="266">
@@ -5249,10 +5246,10 @@
         <v>5</v>
       </c>
       <c r="C266" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D266" t="n">
-        <v>66</v>
+        <v>96</v>
       </c>
     </row>
     <row r="267">
@@ -5263,10 +5260,10 @@
         <v>5</v>
       </c>
       <c r="C267" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D267" t="n">
-        <v>96</v>
+        <v>108</v>
       </c>
     </row>
     <row r="268">
@@ -5277,10 +5274,10 @@
         <v>5</v>
       </c>
       <c r="C268" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D268" t="n">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="269">
@@ -5291,10 +5288,10 @@
         <v>5</v>
       </c>
       <c r="C269" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D269" t="n">
-        <v>110</v>
+        <v>126</v>
       </c>
     </row>
     <row r="270">
@@ -5305,10 +5302,10 @@
         <v>5</v>
       </c>
       <c r="C270" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D270" t="n">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="271">
@@ -5319,10 +5316,10 @@
         <v>5</v>
       </c>
       <c r="C271" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D271" t="n">
-        <v>133</v>
+        <v>223</v>
       </c>
     </row>
     <row r="272">
@@ -5333,10 +5330,10 @@
         <v>5</v>
       </c>
       <c r="C272" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D272" t="n">
-        <v>224</v>
+        <v>276</v>
       </c>
     </row>
     <row r="273">
@@ -5347,10 +5344,10 @@
         <v>5</v>
       </c>
       <c r="C273" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D273" t="n">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="274">
@@ -5361,10 +5358,10 @@
         <v>5</v>
       </c>
       <c r="C274" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D274" t="n">
-        <v>280</v>
+        <v>301</v>
       </c>
     </row>
     <row r="275">
@@ -5375,10 +5372,10 @@
         <v>5</v>
       </c>
       <c r="C275" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D275" t="n">
-        <v>302</v>
+        <v>38</v>
       </c>
     </row>
     <row r="276">
@@ -5389,10 +5386,10 @@
         <v>5</v>
       </c>
       <c r="C276" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D276" t="n">
-        <v>38</v>
+        <v>190</v>
       </c>
     </row>
     <row r="277">
@@ -5403,10 +5400,10 @@
         <v>5</v>
       </c>
       <c r="C277" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D277" t="n">
-        <v>191</v>
+        <v>245</v>
       </c>
     </row>
     <row r="278">
@@ -5417,10 +5414,10 @@
         <v>5</v>
       </c>
       <c r="C278" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D278" t="n">
-        <v>246</v>
+        <v>258</v>
       </c>
     </row>
     <row r="279">
@@ -5431,10 +5428,10 @@
         <v>5</v>
       </c>
       <c r="C279" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D279" t="n">
-        <v>259</v>
+        <v>270</v>
       </c>
     </row>
     <row r="280">
@@ -5442,27 +5439,27 @@
         <v>317</v>
       </c>
       <c r="B280" t="s">
-        <v>5</v>
+        <v>318</v>
       </c>
       <c r="C280" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D280" t="n">
-        <v>271</v>
+        <v>88</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="s">
+        <v>319</v>
+      </c>
+      <c r="B281" t="s">
         <v>318</v>
       </c>
-      <c r="B281" t="s">
-        <v>319</v>
-      </c>
       <c r="C281" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D281" t="n">
-        <v>88</v>
+        <v>109</v>
       </c>
     </row>
     <row r="282">
@@ -5470,13 +5467,13 @@
         <v>320</v>
       </c>
       <c r="B282" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C282" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D282" t="n">
-        <v>109</v>
+        <v>136</v>
       </c>
     </row>
     <row r="283">
@@ -5484,13 +5481,13 @@
         <v>321</v>
       </c>
       <c r="B283" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C283" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D283" t="n">
-        <v>136</v>
+        <v>147</v>
       </c>
     </row>
     <row r="284">
@@ -5498,13 +5495,13 @@
         <v>322</v>
       </c>
       <c r="B284" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C284" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D284" t="n">
-        <v>147</v>
+        <v>179</v>
       </c>
     </row>
     <row r="285">
@@ -5512,13 +5509,13 @@
         <v>323</v>
       </c>
       <c r="B285" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C285" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D285" t="n">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="286">
@@ -5526,13 +5523,13 @@
         <v>324</v>
       </c>
       <c r="B286" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C286" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D286" t="n">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="287">
@@ -5540,13 +5537,13 @@
         <v>325</v>
       </c>
       <c r="B287" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C287" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D287" t="n">
-        <v>186</v>
+        <v>226</v>
       </c>
     </row>
     <row r="288">
@@ -5554,13 +5551,13 @@
         <v>326</v>
       </c>
       <c r="B288" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C288" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D288" t="n">
-        <v>227</v>
+        <v>275</v>
       </c>
     </row>
     <row r="289">
@@ -5568,13 +5565,13 @@
         <v>327</v>
       </c>
       <c r="B289" t="s">
-        <v>319</v>
+        <v>5</v>
       </c>
       <c r="C289" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D289" t="n">
-        <v>276</v>
+        <v>157</v>
       </c>
     </row>
     <row r="290">
@@ -5582,27 +5579,27 @@
         <v>328</v>
       </c>
       <c r="B290" t="s">
-        <v>5</v>
+        <v>329</v>
       </c>
       <c r="C290" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D290" t="n">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="s">
+        <v>330</v>
+      </c>
+      <c r="B291" t="s">
         <v>329</v>
       </c>
-      <c r="B291" t="s">
-        <v>330</v>
-      </c>
       <c r="C291" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D291" t="n">
-        <v>152</v>
+        <v>256</v>
       </c>
     </row>
     <row r="292">
@@ -5610,27 +5607,27 @@
         <v>331</v>
       </c>
       <c r="B292" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C292" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D292" t="n">
-        <v>257</v>
+        <v>87</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="s">
+        <v>333</v>
+      </c>
+      <c r="B293" t="s">
         <v>332</v>
       </c>
-      <c r="B293" t="s">
-        <v>333</v>
-      </c>
       <c r="C293" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D293" t="n">
-        <v>87</v>
+        <v>239</v>
       </c>
     </row>
     <row r="294">
@@ -5638,13 +5635,13 @@
         <v>334</v>
       </c>
       <c r="B294" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C294" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D294" t="n">
-        <v>240</v>
+        <v>84</v>
       </c>
     </row>
     <row r="295">
@@ -5652,27 +5649,27 @@
         <v>335</v>
       </c>
       <c r="B295" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="C295" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D295" t="n">
-        <v>84</v>
+        <v>33</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="s">
+        <v>337</v>
+      </c>
+      <c r="B296" t="s">
         <v>336</v>
       </c>
-      <c r="B296" t="s">
-        <v>337</v>
-      </c>
       <c r="C296" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D296" t="n">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="297">
@@ -5680,13 +5677,13 @@
         <v>338</v>
       </c>
       <c r="B297" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C297" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D297" t="n">
-        <v>138</v>
+        <v>114</v>
       </c>
     </row>
     <row r="298">
@@ -5694,13 +5691,13 @@
         <v>339</v>
       </c>
       <c r="B298" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C298" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D298" t="n">
-        <v>114</v>
+        <v>278</v>
       </c>
     </row>
     <row r="299">
@@ -5708,13 +5705,13 @@
         <v>340</v>
       </c>
       <c r="B299" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C299" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D299" t="n">
-        <v>279</v>
+        <v>82</v>
       </c>
     </row>
     <row r="300">
@@ -5722,13 +5719,13 @@
         <v>341</v>
       </c>
       <c r="B300" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C300" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D300" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="301">
@@ -5736,13 +5733,13 @@
         <v>342</v>
       </c>
       <c r="B301" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C301" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D301" t="n">
-        <v>83</v>
+        <v>58</v>
       </c>
     </row>
     <row r="302">
@@ -5750,13 +5747,13 @@
         <v>343</v>
       </c>
       <c r="B302" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C302" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D302" t="n">
-        <v>58</v>
+        <v>237</v>
       </c>
     </row>
     <row r="303">
@@ -5764,13 +5761,13 @@
         <v>344</v>
       </c>
       <c r="B303" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C303" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D303" t="n">
-        <v>238</v>
+        <v>197</v>
       </c>
     </row>
     <row r="304">
@@ -5778,13 +5775,13 @@
         <v>345</v>
       </c>
       <c r="B304" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C304" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D304" t="n">
-        <v>198</v>
+        <v>144</v>
       </c>
     </row>
     <row r="305">
@@ -5792,13 +5789,13 @@
         <v>346</v>
       </c>
       <c r="B305" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C305" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D305" t="n">
-        <v>144</v>
+        <v>221</v>
       </c>
     </row>
     <row r="306">
@@ -5806,27 +5803,27 @@
         <v>347</v>
       </c>
       <c r="B306" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
       <c r="C306" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D306" t="n">
-        <v>222</v>
+        <v>154</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="s">
+        <v>349</v>
+      </c>
+      <c r="B307" t="s">
         <v>348</v>
       </c>
-      <c r="B307" t="s">
-        <v>349</v>
-      </c>
       <c r="C307" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D307" t="n">
-        <v>154</v>
+        <v>175</v>
       </c>
     </row>
     <row r="308">
@@ -5834,27 +5831,27 @@
         <v>350</v>
       </c>
       <c r="B308" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C308" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D308" t="n">
-        <v>176</v>
+        <v>285</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="s">
+        <v>352</v>
+      </c>
+      <c r="B309" t="s">
         <v>351</v>
       </c>
-      <c r="B309" t="s">
-        <v>352</v>
-      </c>
       <c r="C309" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D309" t="n">
-        <v>286</v>
+        <v>218</v>
       </c>
     </row>
     <row r="310">
@@ -5862,69 +5859,69 @@
         <v>353</v>
       </c>
       <c r="B310" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C310" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D310" t="n">
-        <v>219</v>
+        <v>19</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B311" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C311" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D311" t="n">
-        <v>19</v>
+        <v>56</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B312" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C312" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D312" t="n">
-        <v>56</v>
+        <v>194</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B313" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C313" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D313" t="n">
-        <v>195</v>
+        <v>8</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="s">
+        <v>361</v>
+      </c>
+      <c r="B314" t="s">
         <v>360</v>
       </c>
-      <c r="B314" t="s">
-        <v>361</v>
-      </c>
       <c r="C314" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D314" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="315">
@@ -5932,13 +5929,13 @@
         <v>362</v>
       </c>
       <c r="B315" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C315" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D315" t="n">
-        <v>7</v>
+        <v>214</v>
       </c>
     </row>
     <row r="316">
@@ -5946,13 +5943,13 @@
         <v>363</v>
       </c>
       <c r="B316" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C316" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D316" t="n">
-        <v>215</v>
+        <v>283</v>
       </c>
     </row>
     <row r="317">
@@ -5960,13 +5957,13 @@
         <v>364</v>
       </c>
       <c r="B317" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C317" t="s">
+        <v>298</v>
+      </c>
+      <c r="D317" t="n">
         <v>299</v>
-      </c>
-      <c r="D317" t="n">
-        <v>284</v>
       </c>
     </row>
     <row r="318">
@@ -5974,41 +5971,41 @@
         <v>365</v>
       </c>
       <c r="B318" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="C318" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D318" t="n">
-        <v>300</v>
+        <v>184</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B319" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C319" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D319" t="n">
-        <v>185</v>
+        <v>317</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="s">
+        <v>369</v>
+      </c>
+      <c r="B320" t="s">
         <v>368</v>
       </c>
-      <c r="B320" t="s">
-        <v>369</v>
-      </c>
       <c r="C320" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D320" t="n">
-        <v>318</v>
+        <v>85</v>
       </c>
     </row>
     <row r="321">
@@ -6016,13 +6013,13 @@
         <v>370</v>
       </c>
       <c r="B321" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C321" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D321" t="n">
-        <v>85</v>
+        <v>209</v>
       </c>
     </row>
     <row r="322">
@@ -6030,27 +6027,27 @@
         <v>371</v>
       </c>
       <c r="B322" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C322" t="s">
-        <v>299</v>
+        <v>373</v>
       </c>
       <c r="D322" t="n">
-        <v>210</v>
+        <v>70</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="s">
+        <v>374</v>
+      </c>
+      <c r="B323" t="s">
         <v>372</v>
       </c>
-      <c r="B323" t="s">
+      <c r="C323" t="s">
         <v>373</v>
       </c>
-      <c r="C323" t="s">
-        <v>374</v>
-      </c>
       <c r="D323" t="n">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="324">
@@ -6058,13 +6055,13 @@
         <v>375</v>
       </c>
       <c r="B324" t="s">
+        <v>372</v>
+      </c>
+      <c r="C324" t="s">
         <v>373</v>
       </c>
-      <c r="C324" t="s">
-        <v>374</v>
-      </c>
       <c r="D324" t="n">
-        <v>79</v>
+        <v>98</v>
       </c>
     </row>
     <row r="325">
@@ -6072,13 +6069,13 @@
         <v>376</v>
       </c>
       <c r="B325" t="s">
+        <v>372</v>
+      </c>
+      <c r="C325" t="s">
         <v>373</v>
       </c>
-      <c r="C325" t="s">
-        <v>374</v>
-      </c>
       <c r="D325" t="n">
-        <v>98</v>
+        <v>228</v>
       </c>
     </row>
     <row r="326">
@@ -6086,13 +6083,13 @@
         <v>377</v>
       </c>
       <c r="B326" t="s">
+        <v>372</v>
+      </c>
+      <c r="C326" t="s">
         <v>373</v>
       </c>
-      <c r="C326" t="s">
-        <v>374</v>
-      </c>
       <c r="D326" t="n">
-        <v>229</v>
+        <v>334</v>
       </c>
     </row>
     <row r="327">
@@ -6100,27 +6097,27 @@
         <v>378</v>
       </c>
       <c r="B327" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C327" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="D327" t="n">
-        <v>335</v>
+        <v>140</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="s">
+        <v>380</v>
+      </c>
+      <c r="B328" t="s">
+        <v>372</v>
+      </c>
+      <c r="C328" t="s">
         <v>379</v>
       </c>
-      <c r="B328" t="s">
-        <v>373</v>
-      </c>
-      <c r="C328" t="s">
-        <v>380</v>
-      </c>
       <c r="D328" t="n">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="329">
@@ -6128,13 +6125,13 @@
         <v>381</v>
       </c>
       <c r="B329" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C329" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D329" t="n">
-        <v>131</v>
+        <v>212</v>
       </c>
     </row>
     <row r="330">
@@ -6142,13 +6139,13 @@
         <v>382</v>
       </c>
       <c r="B330" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C330" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D330" t="n">
-        <v>213</v>
+        <v>186</v>
       </c>
     </row>
     <row r="331">
@@ -6156,13 +6153,13 @@
         <v>383</v>
       </c>
       <c r="B331" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C331" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D331" t="n">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="332">
@@ -6170,41 +6167,41 @@
         <v>384</v>
       </c>
       <c r="B332" t="s">
-        <v>373</v>
+        <v>385</v>
       </c>
       <c r="C332" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D332" t="n">
-        <v>182</v>
+        <v>148</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B333" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C333" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D333" t="n">
-        <v>148</v>
+        <v>51</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="s">
+        <v>388</v>
+      </c>
+      <c r="B334" t="s">
         <v>387</v>
       </c>
-      <c r="B334" t="s">
-        <v>388</v>
-      </c>
       <c r="C334" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D334" t="n">
-        <v>51</v>
+        <v>65</v>
       </c>
     </row>
     <row r="335">
@@ -6212,27 +6209,27 @@
         <v>389</v>
       </c>
       <c r="B335" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C335" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D335" t="n">
-        <v>65</v>
+        <v>115</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="s">
+        <v>391</v>
+      </c>
+      <c r="B336" t="s">
         <v>390</v>
       </c>
-      <c r="B336" t="s">
-        <v>391</v>
-      </c>
       <c r="C336" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D336" t="n">
-        <v>115</v>
+        <v>318</v>
       </c>
     </row>
     <row r="337">
@@ -6240,13 +6237,13 @@
         <v>392</v>
       </c>
       <c r="B337" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C337" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D337" t="n">
-        <v>319</v>
+        <v>227</v>
       </c>
     </row>
     <row r="338">
@@ -6254,27 +6251,13 @@
         <v>393</v>
       </c>
       <c r="B338" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="C338" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D338" t="n">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="339">
-      <c r="A339" t="s">
-        <v>394</v>
-      </c>
-      <c r="B339" t="s">
-        <v>395</v>
-      </c>
-      <c r="C339" t="s">
-        <v>380</v>
-      </c>
-      <c r="D339" t="n">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>